<commit_message>
Completed until Seek bar
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>UserName</t>
   </si>
@@ -100,6 +100,57 @@
   </si>
   <si>
     <t>daaliaexample23@outlook.com</t>
+  </si>
+  <si>
+    <t>Preference</t>
+  </si>
+  <si>
+    <t>Relationship</t>
+  </si>
+  <si>
+    <t>Intent</t>
+  </si>
+  <si>
+    <t>Smokers/Not (Yes/NO)</t>
+  </si>
+  <si>
+    <t>Date with who have kids? (Yes/No)</t>
+  </si>
+  <si>
+    <t>Dating</t>
+  </si>
+  <si>
+    <t>I want to date but nothing serious</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Occupation</t>
+  </si>
+  <si>
+    <t>Job</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Associate's degree</t>
+  </si>
+  <si>
+    <t>AUDhyyg554$$$</t>
+  </si>
+  <si>
+    <t>Women</t>
+  </si>
+  <si>
+    <t>Men</t>
+  </si>
+  <si>
+    <t>fasila48569</t>
+  </si>
+  <si>
+    <t>fahadfazil34267@outlook.com</t>
   </si>
 </sst>
 </file>
@@ -439,20 +490,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K2:K3"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -492,8 +554,29 @@
       <c r="M1" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -525,16 +608,37 @@
         <v>82722</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="L2" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="M2" t="s">
-        <v>24</v>
+        <v>39</v>
+      </c>
+      <c r="N2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -573,6 +677,27 @@
       </c>
       <c r="M3" t="s">
         <v>24</v>
+      </c>
+      <c r="N3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" t="s">
+        <v>34</v>
+      </c>
+      <c r="S3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T3" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>